<commit_message>
Added "Estimated Year Level" for chatbot
</commit_message>
<xml_diff>
--- a/gutenberg-scrape/Gutenberg-Predictions/gutenberg-predictions-all-xlsx.xlsx
+++ b/gutenberg-scrape/Gutenberg-Predictions/gutenberg-predictions-all-xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Engineering\MSA Phase 2 Project\gutenberg-scrape\Gutenberg-Predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19663ED7-F43D-4D05-9DEA-9F7BF91959F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6E0E99-852A-4828-820F-D4A68FCE3A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19432,8 +19432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L104" sqref="L104"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19978,7 +19978,7 @@
       </c>
       <c r="T8" s="8">
         <f>COUNTIF(Table1[Year Level], "Year 12")</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -20052,7 +20052,7 @@
       </c>
       <c r="T9" s="8">
         <f>COUNTIF(Table1[Year Level], "Year 13")</f>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -20126,7 +20126,7 @@
       </c>
       <c r="T10" s="8">
         <f>COUNTIF(Table1[Year Level], "Year 13+")</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -24219,7 +24219,7 @@
       </c>
       <c r="Q71" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13</v>
+        <v>Year 12</v>
       </c>
       <c r="R71"/>
     </row>
@@ -24286,7 +24286,7 @@
       </c>
       <c r="Q72" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13</v>
+        <v>Year 12</v>
       </c>
       <c r="R72"/>
     </row>
@@ -24353,7 +24353,7 @@
       </c>
       <c r="Q73" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13</v>
+        <v>Year 12</v>
       </c>
       <c r="R73"/>
     </row>
@@ -24420,7 +24420,7 @@
       </c>
       <c r="Q74" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13</v>
+        <v>Year 12</v>
       </c>
       <c r="R74"/>
     </row>
@@ -24487,7 +24487,7 @@
       </c>
       <c r="Q75" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13</v>
+        <v>Year 12</v>
       </c>
       <c r="R75"/>
     </row>
@@ -25021,7 +25021,7 @@
       </c>
       <c r="Q83" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13+</v>
+        <v>Year 13</v>
       </c>
       <c r="R83"/>
     </row>
@@ -25088,7 +25088,7 @@
       </c>
       <c r="Q84" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Year 13+</v>
+        <v>Year 13</v>
       </c>
       <c r="R84"/>
     </row>
@@ -26280,7 +26280,7 @@
         <v>296</v>
       </c>
       <c r="C109" s="13">
-        <v>-1.6</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="110" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -26288,7 +26288,7 @@
         <v>297</v>
       </c>
       <c r="C110" s="15">
-        <v>-2.1</v>
+        <v>-2.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>